<commit_message>
update to role distribution
</commit_message>
<xml_diff>
--- a/Role Distribution.xlsx
+++ b/Role Distribution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexborden/Desktop/stroke_prediction_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CFC69D-E037-A44C-B63A-0A5C8938C1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D4459E-A2D4-D54D-9FF6-91954FDF4231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23420" yWindow="-1980" windowWidth="23420" windowHeight="19460" xr2:uid="{DCA70308-FC54-D54A-827D-9C597C8BD600}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{DCA70308-FC54-D54A-827D-9C597C8BD600}"/>
   </bookViews>
   <sheets>
     <sheet name="Role Distrubtion" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
 create visuals to accompany the data story.)</t>
   </si>
   <si>
-    <t>Triangle ( Transform the mockup database into a full database that integrates with your work.)</t>
-  </si>
-  <si>
     <t>X (Perform a quality assurance check on 
 project deliverables against rubric requirements, and test the code.</t>
   </si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Square (Repository/Presentation)</t>
+  </si>
+  <si>
+    <t>Triangle (Transform the mockup database into a full database that integrates with your work.)</t>
   </si>
 </sst>
 </file>
@@ -180,13 +180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2144D4C-F346-404F-80FF-0A99102D0BC2}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,7 +668,7 @@
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" customWidth="1"/>
-    <col min="5" max="5" width="64.5" customWidth="1"/>
+    <col min="5" max="5" width="54.6640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
@@ -696,16 +699,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
@@ -713,16 +716,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -730,16 +733,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="98" customHeight="1" x14ac:dyDescent="0.2">
@@ -749,14 +752,14 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>